<commit_message>
update assembly order template
</commit_message>
<xml_diff>
--- a/ExcelFiles/Templates/assemblyOrderTemplate.xlsx
+++ b/ExcelFiles/Templates/assemblyOrderTemplate.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="15240" activeTab="1"/>
+    <workbookView xWindow="2020" yWindow="1980" windowWidth="28800" windowHeight="15240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="©" sheetId="3" r:id="rId1"/>
     <sheet name="template" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">template!$A$1:$G$49</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">template!$A$1:$G$40</definedName>
     <definedName name="valuevx">42.314159</definedName>
     <definedName name="vertex42_copyright" hidden="1">"© 2010-2014 Vertex42 LLC"</definedName>
     <definedName name="vertex42_id" hidden="1">"packing-slip.xlsx"</definedName>
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>[42]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Packing Slip Template</t>
   </si>
@@ -59,57 +56,53 @@
     <t>Do not delete this worksheet</t>
   </si>
   <si>
-    <t>151 Cheshire Lane N</t>
-  </si>
-  <si>
-    <t>Suite 400</t>
-  </si>
-  <si>
-    <t>Plymouth, MN 55441</t>
-  </si>
-  <si>
     <t>Phone: (321) 752-4130</t>
   </si>
   <si>
     <t>Website: www.glaciertek.com</t>
   </si>
   <si>
-    <t>Total:</t>
-  </si>
-  <si>
-    <t>WWW.glaciertek.com</t>
-  </si>
-  <si>
     <t>Assembly Order</t>
   </si>
   <si>
-    <t>Date Issued</t>
-  </si>
-  <si>
-    <t>Product</t>
-  </si>
-  <si>
-    <t>Assembly Parts</t>
-  </si>
-  <si>
-    <t>Qty</t>
-  </si>
-  <si>
     <t>Date Completed:</t>
   </si>
   <si>
     <t>Assembler:</t>
+  </si>
+  <si>
+    <t>www.glaciertek.com</t>
+  </si>
+  <si>
+    <t>Date Issued:</t>
+  </si>
+  <si>
+    <t>4232 Park Glen Rd</t>
+  </si>
+  <si>
+    <t>St Louis Park, MN 55416</t>
+  </si>
+  <si>
+    <t>Product:</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Package Quantity</t>
+  </si>
+  <si>
+    <t>Order Quantity</t>
+  </si>
+  <si>
+    <t>Quantity:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-  </numFmts>
-  <fonts count="46" x14ac:knownFonts="1">
+  <fonts count="41" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Trebuchet MS"/>
@@ -246,13 +239,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <name val="Trebuchet MS"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <i/>
       <sz val="12"/>
       <name val="Trebuchet MS"/>
@@ -266,21 +252,6 @@
       <scheme val="major"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="28"/>
-      <color theme="4" tint="0.39997558519241921"/>
-      <name val="Arial"/>
-      <family val="1"/>
-      <scheme val="major"/>
-    </font>
-    <font>
       <sz val="18"/>
       <color theme="4"/>
       <name val="Arial"/>
@@ -312,13 +283,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="1"/>
-      <color indexed="9"/>
-      <name val="Trebuchet MS"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="16"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -332,33 +296,10 @@
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Trebuchet MS"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color rgb="FF212121"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="major"/>
     </font>
     <font>
       <sz val="11.5"/>
@@ -386,21 +327,41 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF212121"/>
-      <name val="Trebuchet MS"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Trebuchet MS"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <name val="Trebuchet MS"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="21">
@@ -641,17 +602,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color auto="1"/>
@@ -746,9 +696,31 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -760,21 +732,8 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="46">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -826,9 +785,14 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="44" fontId="34" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -836,239 +800,154 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="18" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="20" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="20" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="34" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="34" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="24" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="34" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="38" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="38" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="38" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="38" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="39" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="39" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="39" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="39" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="39" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="24" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="46">
+  <cellStyles count="51">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
@@ -1096,8 +975,13 @@
     <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Currency" xfId="45" builtinId="4"/>
     <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
@@ -1538,7 +1422,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:D20"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1551,7 +1435,7 @@
     <row r="1" spans="1:3" ht="32" customHeight="1">
       <c r="A1" s="5"/>
       <c r="B1" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="5"/>
     </row>
@@ -1563,14 +1447,14 @@
     <row r="3" spans="1:3" ht="15">
       <c r="A3" s="5"/>
       <c r="B3" s="12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5"/>
       <c r="B4" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -1582,7 +1466,7 @@
     <row r="6" spans="1:3" ht="15">
       <c r="A6" s="5"/>
       <c r="B6" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="5"/>
     </row>
@@ -1594,7 +1478,7 @@
     <row r="8" spans="1:3" ht="30">
       <c r="A8" s="5"/>
       <c r="B8" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="5"/>
     </row>
@@ -1606,7 +1490,7 @@
     <row r="10" spans="1:3" ht="30">
       <c r="A10" s="5"/>
       <c r="B10" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="5"/>
     </row>
@@ -1618,7 +1502,7 @@
     <row r="12" spans="1:3" ht="30">
       <c r="A12" s="5"/>
       <c r="B12" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" s="5"/>
     </row>
@@ -1629,8 +1513,8 @@
     </row>
     <row r="14" spans="1:3" ht="15">
       <c r="A14" s="5"/>
-      <c r="B14" s="22" t="s">
-        <v>7</v>
+      <c r="B14" s="15" t="s">
+        <v>6</v>
       </c>
       <c r="C14" s="5"/>
     </row>
@@ -1641,8 +1525,8 @@
     </row>
     <row r="16" spans="1:3" ht="15">
       <c r="A16" s="5"/>
-      <c r="B16" s="23" t="s">
-        <v>9</v>
+      <c r="B16" s="16" t="s">
+        <v>8</v>
       </c>
       <c r="C16" s="5"/>
     </row>
@@ -1707,7 +1591,7 @@
       <c r="C28" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="45" type="noConversion"/>
+  <phoneticPr fontId="35" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1"/>
     <hyperlink ref="B14" r:id="rId2"/>
@@ -1728,76 +1612,87 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="11.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="27.1640625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="40" customHeight="1">
-      <c r="A1" s="19"/>
+      <c r="A1" s="14"/>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="33" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="D1" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="24" t="s">
+      <c r="C2" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="27">
+      <c r="D2" s="40"/>
+      <c r="E2" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="46"/>
+      <c r="G2" s="41">
         <f ca="1">TODAY()</f>
         <v>43475</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" ht="15" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="C3" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="42"/>
+      <c r="E3" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="47"/>
+      <c r="G3" s="57"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="47"/>
+      <c r="G4" s="58"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1806,10 +1701,8 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
+    <row r="6" spans="1:9" ht="7" customHeight="1">
+      <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1817,468 +1710,357 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" ht="15">
-      <c r="A8" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" ht="15">
-      <c r="A9" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="15">
-      <c r="A10" s="42"/>
-      <c r="B10" s="3"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" ht="15">
-      <c r="A11" s="42"/>
-      <c r="B11" s="3"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" ht="15">
-      <c r="A12" s="44"/>
-      <c r="B12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" ht="13">
-      <c r="A13" s="42"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A15" s="69" t="s">
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="18">
+      <c r="A7" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="82" t="s">
+      <c r="B7" s="34"/>
+      <c r="C7" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="82"/>
-      <c r="D15" s="82"/>
-      <c r="E15" s="28" t="s">
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="I15" s="35"/>
-    </row>
-    <row r="16" spans="1:9" s="51" customFormat="1" ht="51.75" customHeight="1">
-      <c r="A16" s="67"/>
-      <c r="B16" s="83"/>
-      <c r="C16" s="83"/>
-      <c r="D16" s="83"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="54"/>
-      <c r="I16" s="52"/>
-    </row>
-    <row r="17" spans="1:9" ht="27" customHeight="1">
-      <c r="A17" s="68"/>
-      <c r="B17" s="84"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="36"/>
-      <c r="I17" s="43"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="68"/>
-      <c r="B18" s="85"/>
-      <c r="C18" s="85"/>
-      <c r="D18" s="85"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="30"/>
-    </row>
-    <row r="19" spans="1:9" s="51" customFormat="1" ht="59.25" customHeight="1">
-      <c r="A19" s="67"/>
-      <c r="B19" s="83"/>
-      <c r="C19" s="83"/>
-      <c r="D19" s="83"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="60"/>
-      <c r="I19" s="61"/>
-    </row>
-    <row r="20" spans="1:9" s="62" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A20" s="63"/>
-      <c r="B20" s="86"/>
-      <c r="C20" s="87"/>
-      <c r="D20" s="87"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="65"/>
-      <c r="I20" s="66"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="29"/>
-      <c r="B21" s="76"/>
-      <c r="C21" s="76"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="30"/>
-    </row>
-    <row r="22" spans="1:9" ht="60" customHeight="1">
-      <c r="A22" s="56"/>
-      <c r="B22" s="88"/>
-      <c r="C22" s="89"/>
-      <c r="D22" s="89"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="60"/>
-      <c r="I22" s="44"/>
-    </row>
-    <row r="23" spans="1:9" s="62" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A23" s="63"/>
-      <c r="B23" s="86"/>
-      <c r="C23" s="87"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="65"/>
-      <c r="I23" s="66"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="56"/>
-      <c r="B24" s="57"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="30"/>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="29"/>
-      <c r="B25" s="76"/>
-      <c r="C25" s="76"/>
-      <c r="D25" s="76"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="30"/>
-    </row>
-    <row r="26" spans="1:9" ht="60" customHeight="1">
-      <c r="A26" s="56"/>
-      <c r="B26" s="88"/>
-      <c r="C26" s="89"/>
-      <c r="D26" s="89"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="60"/>
-      <c r="I26" s="44"/>
-    </row>
-    <row r="27" spans="1:9" s="62" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A27" s="63"/>
-      <c r="B27" s="86"/>
-      <c r="C27" s="87"/>
-      <c r="D27" s="87"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="65"/>
-      <c r="I27" s="66"/>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="29"/>
-      <c r="B28" s="76"/>
-      <c r="C28" s="76"/>
-      <c r="D28" s="76"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="30"/>
-    </row>
-    <row r="29" spans="1:9" ht="60" customHeight="1">
-      <c r="A29" s="56"/>
-      <c r="B29" s="88"/>
-      <c r="C29" s="89"/>
-      <c r="D29" s="89"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="60"/>
-      <c r="I29" s="44"/>
-    </row>
-    <row r="30" spans="1:9" s="62" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A30" s="63"/>
-      <c r="B30" s="86"/>
-      <c r="C30" s="87"/>
-      <c r="D30" s="87"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="65"/>
-      <c r="I30" s="66"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="29"/>
-      <c r="B31" s="76"/>
-      <c r="C31" s="76"/>
-      <c r="D31" s="76"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="30"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="31"/>
-      <c r="B32" s="81"/>
-      <c r="C32" s="81"/>
-      <c r="D32" s="81"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="21"/>
-    </row>
-    <row r="33" spans="1:9" ht="18" customHeight="1">
-      <c r="A33" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E33" s="37">
-        <f>SUM(E16:E32)</f>
-        <v>0</v>
-      </c>
-      <c r="F33" s="18"/>
-      <c r="G33" s="34">
-        <f>SUM(G16:G32)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" spans="1:9" ht="18" customHeight="1">
-      <c r="A35" s="72"/>
-      <c r="B35" s="73"/>
-      <c r="C35" s="73"/>
-      <c r="D35" s="73"/>
-      <c r="E35" s="73"/>
-      <c r="F35" s="73"/>
-      <c r="G35" s="74"/>
-      <c r="I35" s="44"/>
-    </row>
-    <row r="36" spans="1:9" ht="15">
-      <c r="A36" s="44"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="39"/>
-      <c r="I36" s="44"/>
-    </row>
-    <row r="37" spans="1:9" s="2" customFormat="1" ht="15">
-      <c r="A37" s="44"/>
-      <c r="B37" s="44"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="40"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="45"/>
-    </row>
-    <row r="38" spans="1:9" s="2" customFormat="1" ht="15">
-      <c r="A38" s="44"/>
-      <c r="B38" s="44"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="40"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="45"/>
-    </row>
-    <row r="39" spans="1:9" s="2" customFormat="1" ht="15">
-      <c r="A39" s="44"/>
-      <c r="B39" s="44"/>
-      <c r="C39" s="44"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="40"/>
-      <c r="F39" s="40"/>
-      <c r="G39" s="41"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="45"/>
-    </row>
-    <row r="40" spans="1:9" s="2" customFormat="1" ht="15">
-      <c r="A40" s="44"/>
-      <c r="B40" s="44"/>
-      <c r="C40" s="44"/>
-      <c r="D40" s="40"/>
-      <c r="E40" s="40"/>
-      <c r="F40" s="40"/>
-      <c r="G40" s="41"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="45"/>
-    </row>
-    <row r="41" spans="1:9" s="2" customFormat="1" ht="15">
-      <c r="A41" s="49"/>
-      <c r="B41" s="44"/>
-      <c r="C41" s="44"/>
-      <c r="D41" s="40"/>
-      <c r="E41" s="40"/>
-      <c r="F41" s="40"/>
-      <c r="G41" s="41"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="45"/>
-    </row>
-    <row r="42" spans="1:9" s="2" customFormat="1" ht="15">
-      <c r="A42" s="49"/>
-      <c r="B42" s="44"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="40"/>
-      <c r="F42" s="40"/>
-      <c r="G42" s="41"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="45"/>
-    </row>
-    <row r="43" spans="1:9" s="2" customFormat="1" ht="15">
-      <c r="A43" s="47"/>
-      <c r="B43" s="44"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="40"/>
-      <c r="E43" s="40"/>
-      <c r="F43" s="40"/>
-      <c r="G43" s="41"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="45"/>
-    </row>
-    <row r="44" spans="1:9" s="2" customFormat="1" ht="15">
-      <c r="A44" s="50"/>
-      <c r="B44" s="44"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="40"/>
-      <c r="E44" s="40"/>
-      <c r="F44" s="40"/>
-      <c r="G44" s="41"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="45"/>
-    </row>
-    <row r="45" spans="1:9" s="2" customFormat="1">
-      <c r="A45" s="75"/>
-      <c r="B45" s="76"/>
-      <c r="C45" s="76"/>
-      <c r="D45" s="76"/>
-      <c r="E45" s="76"/>
-      <c r="F45" s="76"/>
-      <c r="G45" s="77"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="46"/>
-    </row>
-    <row r="46" spans="1:9" s="2" customFormat="1">
-      <c r="A46" s="78"/>
-      <c r="B46" s="79"/>
-      <c r="C46" s="79"/>
-      <c r="D46" s="79"/>
-      <c r="E46" s="79"/>
-      <c r="F46" s="79"/>
-      <c r="G46" s="80"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="47"/>
-    </row>
-    <row r="47" spans="1:9" s="2" customFormat="1">
-      <c r="A47" s="16"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="48"/>
-    </row>
-    <row r="48" spans="1:9" ht="15">
-      <c r="A48" s="70" t="s">
-        <v>16</v>
-      </c>
-      <c r="B48" s="71"/>
-      <c r="C48" s="71"/>
-      <c r="D48" s="71"/>
-      <c r="E48" s="71"/>
-      <c r="F48" s="71"/>
-      <c r="G48" s="71"/>
-      <c r="I48" s="44"/>
+      <c r="G7" s="38"/>
+      <c r="I7" s="18"/>
+    </row>
+    <row r="8" spans="1:9" s="24" customFormat="1" ht="20">
+      <c r="A8" s="43"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="51"/>
+      <c r="I8" s="25"/>
+    </row>
+    <row r="9" spans="1:9" s="26" customFormat="1" ht="20" customHeight="1">
+      <c r="A9" s="35"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="52"/>
+      <c r="I9" s="27"/>
+    </row>
+    <row r="10" spans="1:9" s="28" customFormat="1" ht="20">
+      <c r="A10" s="35"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="52"/>
+      <c r="I10" s="27"/>
+    </row>
+    <row r="11" spans="1:9" ht="20">
+      <c r="A11" s="35"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="52"/>
+    </row>
+    <row r="12" spans="1:9" ht="20">
+      <c r="A12" s="35"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="52"/>
+      <c r="I12" s="19"/>
+    </row>
+    <row r="13" spans="1:9" ht="20">
+      <c r="A13" s="35"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="52"/>
+      <c r="I13" s="19"/>
+    </row>
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="20">
+      <c r="A14" s="35"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="20"/>
+    </row>
+    <row r="15" spans="1:9" s="2" customFormat="1" ht="20">
+      <c r="A15" s="35"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="20"/>
+    </row>
+    <row r="16" spans="1:9" s="2" customFormat="1" ht="20">
+      <c r="A16" s="35"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="20"/>
+    </row>
+    <row r="17" spans="1:9" s="2" customFormat="1" ht="20">
+      <c r="A17" s="35"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="20"/>
+    </row>
+    <row r="18" spans="1:9" s="2" customFormat="1" ht="20">
+      <c r="A18" s="35"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="20"/>
+    </row>
+    <row r="19" spans="1:9" s="2" customFormat="1" ht="20">
+      <c r="A19" s="35"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="20"/>
+    </row>
+    <row r="20" spans="1:9" s="2" customFormat="1" ht="20">
+      <c r="A20" s="35"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="20"/>
+    </row>
+    <row r="21" spans="1:9" s="2" customFormat="1" ht="20">
+      <c r="A21" s="35"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="21"/>
+    </row>
+    <row r="22" spans="1:9" s="2" customFormat="1" ht="20">
+      <c r="A22" s="35"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="22"/>
+    </row>
+    <row r="23" spans="1:9" s="2" customFormat="1" ht="20">
+      <c r="A23" s="35"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="23"/>
+    </row>
+    <row r="24" spans="1:9" ht="20">
+      <c r="A24" s="35"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="52"/>
+      <c r="I24" s="19"/>
+    </row>
+    <row r="25" spans="1:9" ht="20">
+      <c r="A25" s="35"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="52"/>
+    </row>
+    <row r="26" spans="1:9" ht="20">
+      <c r="A26" s="35"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="52"/>
+    </row>
+    <row r="27" spans="1:9" ht="20">
+      <c r="A27" s="35"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="52"/>
+    </row>
+    <row r="28" spans="1:9" ht="20">
+      <c r="A28" s="35"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="52"/>
+    </row>
+    <row r="29" spans="1:9" ht="20">
+      <c r="A29" s="35"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="52"/>
+    </row>
+    <row r="30" spans="1:9" ht="20">
+      <c r="A30" s="35"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="52"/>
+    </row>
+    <row r="31" spans="1:9" ht="20">
+      <c r="A31" s="35"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="52"/>
+    </row>
+    <row r="32" spans="1:9" ht="20">
+      <c r="A32" s="35"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="52"/>
+    </row>
+    <row r="33" spans="1:7" ht="20">
+      <c r="A33" s="35"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="52"/>
+    </row>
+    <row r="34" spans="1:7" ht="20">
+      <c r="A34" s="35"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="52"/>
+    </row>
+    <row r="35" spans="1:7" ht="20">
+      <c r="A35" s="35"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="52"/>
+    </row>
+    <row r="36" spans="1:7" ht="20">
+      <c r="A36" s="35"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="52"/>
+    </row>
+    <row r="37" spans="1:7" ht="20">
+      <c r="A37" s="35"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="52"/>
+    </row>
+    <row r="38" spans="1:7" ht="20">
+      <c r="A38" s="53"/>
+      <c r="B38" s="54"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="55"/>
+      <c r="G38" s="56"/>
+    </row>
+    <row r="39" spans="1:7" ht="15">
+      <c r="A39" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="A48:G48"/>
-    <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="B32:D32"/>
+  <mergeCells count="9">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <phoneticPr fontId="45" type="noConversion"/>
+  <phoneticPr fontId="35" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A48" r:id="rId1"/>
+    <hyperlink ref="A39" r:id="rId1"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.25" header="0.5" footer="0.25"/>
-  <pageSetup scale="71" fitToHeight="0" orientation="portrait"/>
+  <pageSetup scale="93" fitToHeight="0" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
   <extLst>

</xml_diff>

<commit_message>
populate assembly file with relevant data
</commit_message>
<xml_diff>
--- a/ExcelFiles/Templates/assemblyOrderTemplate.xlsx
+++ b/ExcelFiles/Templates/assemblyOrderTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="10200" yWindow="0" windowWidth="17740" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="©" sheetId="2" r:id="rId1"/>
@@ -95,7 +95,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -163,6 +163,15 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -178,7 +187,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -272,43 +281,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -316,30 +338,60 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -672,7 +724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -683,7 +735,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:2" ht="21">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
@@ -698,22 +750,22 @@
       </c>
     </row>
     <row r="6" spans="2:2">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="30">
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="30">
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:2" ht="30">
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -723,7 +775,7 @@
       </c>
     </row>
     <row r="16" spans="2:2">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -745,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -761,380 +813,470 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="40" customHeight="1">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6" t="s">
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="7"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="12">
+      <c r="F2" s="24"/>
+      <c r="G2" s="5">
         <f ca="1" xml:space="preserve"> TODAY()</f>
         <v>43476</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="24"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="13"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="11" t="s">
+      <c r="C4" s="21"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="13"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" ht="7" customHeight="1">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" ht="19" customHeight="1">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="23" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23" t="s">
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="24"/>
+      <c r="G7" s="28"/>
     </row>
     <row r="8" spans="1:7" ht="19" customHeight="1">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="17"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12" t="str">
+        <f>IF($D8="","",$D8*$D$4)</f>
+        <v/>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="19" customHeight="1">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="17"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15" t="str">
+        <f t="shared" ref="G9:G37" si="0">IF($D9="","",$D9*$D$4)</f>
+        <v/>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="19" customHeight="1">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="17"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="19" customHeight="1">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="19" customHeight="1">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="17"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="19" customHeight="1">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="17"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="19" customHeight="1">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="17"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="19" customHeight="1">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="17"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="19" customHeight="1">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="17"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="19" customHeight="1">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="17"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="19" customHeight="1">
-      <c r="A18" s="15"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="17"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="19" customHeight="1">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="17"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="19" customHeight="1">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="17"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="19" customHeight="1">
-      <c r="A21" s="15"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="17"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="19" customHeight="1">
-      <c r="A22" s="15"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="17"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="19" customHeight="1">
-      <c r="A23" s="15"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="17"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="19" customHeight="1">
-      <c r="A24" s="15"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="17"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="19" customHeight="1">
-      <c r="A25" s="15"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="17"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="19" customHeight="1">
-      <c r="A26" s="15"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="17"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="19" customHeight="1">
-      <c r="A27" s="15"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="17"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="19" customHeight="1">
-      <c r="A28" s="15"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="17"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="19" customHeight="1">
-      <c r="A29" s="15"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="17"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="19" customHeight="1">
-      <c r="A30" s="15"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="17"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="19" customHeight="1">
-      <c r="A31" s="15"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="17"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="19" customHeight="1">
-      <c r="A32" s="15"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="17"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="19" customHeight="1">
-      <c r="A33" s="15"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="17"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="19" customHeight="1">
-      <c r="A34" s="15"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="17"/>
+      <c r="A34" s="13"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="19" customHeight="1">
-      <c r="A35" s="15"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="17"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="19" customHeight="1">
-      <c r="A36" s="15"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="17"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="19" customHeight="1">
-      <c r="A37" s="18"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="20"/>
+      <c r="A37" s="16"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
     <mergeCell ref="A38:G38"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -1146,6 +1288,8 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="F7:G7"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D2:D3"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
deal with print margins
</commit_message>
<xml_diff>
--- a/ExcelFiles/Templates/assemblyOrderTemplate.xlsx
+++ b/ExcelFiles/Templates/assemblyOrderTemplate.xlsx
@@ -795,16 +795,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="3.83203125" customWidth="1"/>
     <col min="3" max="3" width="7.83203125" customWidth="1"/>
     <col min="4" max="4" width="15.83203125" customWidth="1"/>
     <col min="5" max="5" width="9.83203125" customWidth="1"/>
@@ -924,7 +924,7 @@
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="15" t="str">
-        <f t="shared" ref="G9:G37" si="0">IF($D9="","",$D9*$D$4)</f>
+        <f t="shared" ref="G9:G33" si="0">IF($D9="","",$D9*$D$4)</f>
         <v/>
       </c>
     </row>
@@ -1205,79 +1205,31 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="19" customHeight="1">
-      <c r="A33" s="13"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="19" customHeight="1">
-      <c r="A34" s="13"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="19" customHeight="1">
-      <c r="A35" s="13"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="19" customHeight="1">
-      <c r="A36" s="13"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="19" customHeight="1">
-      <c r="A37" s="16"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="19" t="s">
+      <c r="A33" s="16"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="A34:G34"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="C1:F1"/>
@@ -1293,7 +1245,7 @@
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A38" r:id="rId1"/>
+    <hyperlink ref="A34" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.25" header="0.5" footer="0.25"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>